<commit_message>
membuat 2 tombol perhitungan knn,  menyempurnakan code di controller untuk kedua tombol dan memperbaiki tampilan sweet alert perhitungan knn
</commit_message>
<xml_diff>
--- a/Perhitungan K-NN.xlsx
+++ b/Perhitungan K-NN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Project\Knn-game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BF5345-3FF7-43FE-A0CE-70D26FDEEA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{382EBBCB-D4F0-4194-8E51-ACBEF864AE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8976" firstSheet="1" activeTab="5" xr2:uid="{9D91D5F0-3A53-429C-B84E-A3FB8A72F2C8}"/>
   </bookViews>
@@ -29,6 +29,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Tambah!$L$2:$N$8</definedName>
   </definedNames>
   <calcPr calcId="181029" iterate="1"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -231,7 +232,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#0\ &quot;%&quot;"/>
-    <numFmt numFmtId="166" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -799,7 +800,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -842,28 +843,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -885,23 +904,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1555,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C9DAB6-9546-44E5-B64E-4436F608C268}">
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2172,7 +2174,7 @@
       </c>
       <c r="I13" s="1">
         <f>Tambah!$B10</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J13" s="1">
         <f>Tambah!$B11</f>
@@ -2190,7 +2192,7 @@
   <dimension ref="A3:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2273,7 +2275,7 @@
       </c>
       <c r="I5">
         <f>MIN('Data Latih'!I$2:I$11,'Data Latih'!I$13)</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J5">
         <f>MIN('Data Latih'!J$2:J$11,'Data Latih'!J$13)</f>
@@ -2921,154 +2923,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="str">
+      <c r="A1" s="43" t="str">
         <f>Normalisasi!A1</f>
         <v>No</v>
       </c>
-      <c r="B1" s="51" t="str">
+      <c r="B1" s="44" t="str">
         <f>Normalisasi!B1</f>
         <v>q1</v>
       </c>
-      <c r="C1" s="51" t="str">
+      <c r="C1" s="44" t="str">
         <f>Normalisasi!C1</f>
         <v>q2</v>
       </c>
-      <c r="D1" s="51" t="str">
+      <c r="D1" s="44" t="str">
         <f>Normalisasi!D1</f>
         <v>q3</v>
       </c>
-      <c r="E1" s="51" t="str">
+      <c r="E1" s="44" t="str">
         <f>Normalisasi!E1</f>
         <v>q4</v>
       </c>
-      <c r="F1" s="51" t="str">
+      <c r="F1" s="44" t="str">
         <f>Normalisasi!F1</f>
         <v>q5</v>
       </c>
-      <c r="G1" s="51" t="str">
+      <c r="G1" s="44" t="str">
         <f>Normalisasi!G1</f>
         <v>q6</v>
       </c>
-      <c r="H1" s="51" t="str">
+      <c r="H1" s="44" t="str">
         <f>Normalisasi!H1</f>
         <v>q7</v>
       </c>
-      <c r="I1" s="51" t="str">
+      <c r="I1" s="44" t="str">
         <f>Normalisasi!I1</f>
         <v>q8</v>
       </c>
-      <c r="J1" s="51" t="str">
+      <c r="J1" s="44" t="str">
         <f>Normalisasi!J1</f>
         <v>q9</v>
       </c>
-      <c r="K1" s="51" t="str">
+      <c r="K1" s="44" t="str">
         <f>Normalisasi!K1</f>
         <v>Kelas</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="45" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="48">
+      <c r="A2" s="41">
         <f>Normalisasi!$A2</f>
         <v>1</v>
       </c>
-      <c r="B2" s="49">
+      <c r="B2" s="42">
         <f>'Data Latih'!B2</f>
         <v>2</v>
       </c>
-      <c r="C2" s="49">
+      <c r="C2" s="42">
         <f>'Data Latih'!C2</f>
         <v>2</v>
       </c>
-      <c r="D2" s="49">
+      <c r="D2" s="42">
         <f>'Data Latih'!D2</f>
         <v>1</v>
       </c>
-      <c r="E2" s="49">
+      <c r="E2" s="42">
         <f>'Data Latih'!E2</f>
         <v>1</v>
       </c>
-      <c r="F2" s="49">
+      <c r="F2" s="42">
         <f>'Data Latih'!F2</f>
         <v>1</v>
       </c>
-      <c r="G2" s="49">
+      <c r="G2" s="42">
         <f>'Data Latih'!G2</f>
         <v>2</v>
       </c>
-      <c r="H2" s="49">
+      <c r="H2" s="42">
         <f>'Data Latih'!H2</f>
         <v>2</v>
       </c>
-      <c r="I2" s="49">
+      <c r="I2" s="42">
         <f>'Data Latih'!I2</f>
         <v>67</v>
       </c>
-      <c r="J2" s="49">
+      <c r="J2" s="42">
         <f>'Data Latih'!J2</f>
         <v>1</v>
       </c>
-      <c r="K2" s="54" t="str">
+      <c r="K2" s="47" t="str">
         <f>'Data Latih'!K2</f>
         <v>Berat</v>
       </c>
-      <c r="L2" s="55" t="str">
+      <c r="L2" s="48" t="str">
         <f>Distance!$C$13</f>
         <v>Berat</v>
       </c>
-      <c r="N2" s="36" t="s">
+      <c r="N2" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="36"/>
+      <c r="O2" s="54"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A3" s="44">
+      <c r="A3" s="37">
         <f>Normalisasi!$A3</f>
         <v>2</v>
       </c>
-      <c r="B3" s="43">
+      <c r="B3" s="36">
         <f>'Data Latih'!B3</f>
         <v>2</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="36">
         <f>'Data Latih'!C3</f>
         <v>1</v>
       </c>
-      <c r="D3" s="43">
+      <c r="D3" s="36">
         <f>'Data Latih'!D3</f>
         <v>2</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="36">
         <f>'Data Latih'!E3</f>
         <v>1</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="36">
         <f>'Data Latih'!F3</f>
         <v>1</v>
       </c>
-      <c r="G3" s="43">
+      <c r="G3" s="36">
         <f>'Data Latih'!G3</f>
         <v>2</v>
       </c>
-      <c r="H3" s="43">
+      <c r="H3" s="36">
         <f>'Data Latih'!H3</f>
         <v>2</v>
       </c>
-      <c r="I3" s="43">
+      <c r="I3" s="36">
         <f>'Data Latih'!I3</f>
         <v>15</v>
       </c>
-      <c r="J3" s="43">
+      <c r="J3" s="36">
         <f>'Data Latih'!J3</f>
         <v>3</v>
       </c>
-      <c r="K3" s="58" t="str">
+      <c r="K3" s="51" t="str">
         <f>'Data Latih'!K3</f>
         <v>Berat</v>
       </c>
-      <c r="L3" s="59" t="str">
+      <c r="L3" s="52" t="str">
         <f>Distance!$G$13</f>
         <v>Ringan</v>
       </c>
@@ -3090,51 +3092,51 @@
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="44">
+      <c r="A4" s="37">
         <f>Normalisasi!$A4</f>
         <v>3</v>
       </c>
-      <c r="B4" s="43">
+      <c r="B4" s="36">
         <f>'Data Latih'!B4</f>
         <v>1</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="36">
         <f>'Data Latih'!C4</f>
         <v>1</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D4" s="36">
         <f>'Data Latih'!D4</f>
         <v>2</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="36">
         <f>'Data Latih'!E4</f>
         <v>1</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="36">
         <f>'Data Latih'!F4</f>
         <v>1</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="36">
         <f>'Data Latih'!G4</f>
         <v>3</v>
       </c>
-      <c r="H4" s="43">
+      <c r="H4" s="36">
         <f>'Data Latih'!H4</f>
         <v>2</v>
       </c>
-      <c r="I4" s="43">
+      <c r="I4" s="36">
         <f>'Data Latih'!I4</f>
         <v>65</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="36">
         <f>'Data Latih'!J4</f>
         <v>2</v>
       </c>
-      <c r="K4" s="43" t="str">
+      <c r="K4" s="36" t="str">
         <f>'Data Latih'!K4</f>
         <v>Ringan</v>
       </c>
-      <c r="L4" s="45" t="str">
+      <c r="L4" s="38" t="str">
         <f>Distance!K13</f>
         <v>Berat</v>
       </c>
@@ -3156,51 +3158,51 @@
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="44">
+      <c r="A5" s="37">
         <f>Normalisasi!$A5</f>
         <v>4</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="36">
         <f>'Data Latih'!B5</f>
         <v>2</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="36">
         <f>'Data Latih'!C5</f>
         <v>2</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="36">
         <f>'Data Latih'!D5</f>
         <v>2</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="36">
         <f>'Data Latih'!E5</f>
         <v>2</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="36">
         <f>'Data Latih'!F5</f>
         <v>2</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="36">
         <f>'Data Latih'!G5</f>
         <v>2</v>
       </c>
-      <c r="H5" s="43">
+      <c r="H5" s="36">
         <f>'Data Latih'!H5</f>
         <v>2</v>
       </c>
-      <c r="I5" s="43">
+      <c r="I5" s="36">
         <f>'Data Latih'!I5</f>
         <v>20</v>
       </c>
-      <c r="J5" s="43">
+      <c r="J5" s="36">
         <f>'Data Latih'!J5</f>
         <v>2</v>
       </c>
-      <c r="K5" s="56" t="str">
+      <c r="K5" s="49" t="str">
         <f>'Data Latih'!K5</f>
         <v>Berat</v>
       </c>
-      <c r="L5" s="57" t="str">
+      <c r="L5" s="50" t="str">
         <f>Distance!$O$13</f>
         <v>Berat</v>
       </c>
@@ -3222,51 +3224,51 @@
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6" s="44">
+      <c r="A6" s="37">
         <f>Normalisasi!$A6</f>
         <v>5</v>
       </c>
-      <c r="B6" s="43">
+      <c r="B6" s="36">
         <f>'Data Latih'!B6</f>
         <v>1</v>
       </c>
-      <c r="C6" s="43">
+      <c r="C6" s="36">
         <f>'Data Latih'!C6</f>
         <v>1</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="36">
         <f>'Data Latih'!D6</f>
         <v>2</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="36">
         <f>'Data Latih'!E6</f>
         <v>3</v>
       </c>
-      <c r="F6" s="43">
+      <c r="F6" s="36">
         <f>'Data Latih'!F6</f>
         <v>3</v>
       </c>
-      <c r="G6" s="43">
+      <c r="G6" s="36">
         <f>'Data Latih'!G6</f>
         <v>3</v>
       </c>
-      <c r="H6" s="43">
+      <c r="H6" s="36">
         <f>'Data Latih'!H6</f>
         <v>1</v>
       </c>
-      <c r="I6" s="43">
+      <c r="I6" s="36">
         <f>'Data Latih'!I6</f>
         <v>18</v>
       </c>
-      <c r="J6" s="43">
+      <c r="J6" s="36">
         <f>'Data Latih'!J6</f>
         <v>3</v>
       </c>
-      <c r="K6" s="43" t="str">
+      <c r="K6" s="36" t="str">
         <f>'Data Latih'!K6</f>
         <v>Ringan</v>
       </c>
-      <c r="L6" s="45" t="str">
+      <c r="L6" s="38" t="str">
         <f>Distance!$S$13</f>
         <v>Berat</v>
       </c>
@@ -3281,152 +3283,152 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A7" s="44">
+      <c r="A7" s="37">
         <f>Normalisasi!$A7</f>
         <v>6</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="36">
         <f>'Data Latih'!B7</f>
         <v>2</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="36">
         <f>'Data Latih'!C7</f>
         <v>1</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="36">
         <f>'Data Latih'!D7</f>
         <v>1</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="36">
         <f>'Data Latih'!E7</f>
         <v>2</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="36">
         <f>'Data Latih'!F7</f>
         <v>3</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="36">
         <f>'Data Latih'!G7</f>
         <v>3</v>
       </c>
-      <c r="H7" s="43">
+      <c r="H7" s="36">
         <f>'Data Latih'!H7</f>
         <v>2</v>
       </c>
-      <c r="I7" s="43">
+      <c r="I7" s="36">
         <f>'Data Latih'!I7</f>
         <v>24</v>
       </c>
-      <c r="J7" s="43">
+      <c r="J7" s="36">
         <f>'Data Latih'!J7</f>
         <v>1</v>
       </c>
-      <c r="K7" s="43" t="str">
+      <c r="K7" s="36" t="str">
         <f>'Data Latih'!K7</f>
         <v>Ringan</v>
       </c>
-      <c r="L7" s="45" t="str">
+      <c r="L7" s="38" t="str">
         <f>Distance!$W$13</f>
         <v>Berat</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8" s="44">
+      <c r="A8" s="37">
         <f>Normalisasi!$A8</f>
         <v>7</v>
       </c>
-      <c r="B8" s="43">
+      <c r="B8" s="36">
         <f>'Data Latih'!B8</f>
         <v>2</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="36">
         <f>'Data Latih'!C8</f>
         <v>2</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D8" s="36">
         <f>'Data Latih'!D8</f>
         <v>2</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="36">
         <f>'Data Latih'!E8</f>
         <v>3</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="36">
         <f>'Data Latih'!F8</f>
         <v>2</v>
       </c>
-      <c r="G8" s="43">
+      <c r="G8" s="36">
         <f>'Data Latih'!G8</f>
         <v>1</v>
       </c>
-      <c r="H8" s="43">
+      <c r="H8" s="36">
         <f>'Data Latih'!H8</f>
         <v>1</v>
       </c>
-      <c r="I8" s="43">
+      <c r="I8" s="36">
         <f>'Data Latih'!I8</f>
         <v>30</v>
       </c>
-      <c r="J8" s="43">
+      <c r="J8" s="36">
         <f>'Data Latih'!J8</f>
         <v>3</v>
       </c>
-      <c r="K8" s="58" t="str">
+      <c r="K8" s="51" t="str">
         <f>'Data Latih'!K8</f>
         <v>Berat</v>
       </c>
-      <c r="L8" s="59" t="str">
+      <c r="L8" s="52" t="str">
         <f>Distance!$AA$13</f>
         <v>Ringan</v>
       </c>
       <c r="M8" s="17"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A9" s="44">
+      <c r="A9" s="37">
         <f>Normalisasi!$A9</f>
         <v>8</v>
       </c>
-      <c r="B9" s="43">
+      <c r="B9" s="36">
         <f>'Data Latih'!B9</f>
         <v>2</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="36">
         <f>'Data Latih'!C9</f>
         <v>1</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="36">
         <f>'Data Latih'!D9</f>
         <v>2</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="36">
         <f>'Data Latih'!E9</f>
         <v>3</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="36">
         <f>'Data Latih'!F9</f>
         <v>1</v>
       </c>
-      <c r="G9" s="43">
+      <c r="G9" s="36">
         <f>'Data Latih'!G9</f>
         <v>3</v>
       </c>
-      <c r="H9" s="43">
+      <c r="H9" s="36">
         <f>'Data Latih'!H9</f>
         <v>2</v>
       </c>
-      <c r="I9" s="43">
+      <c r="I9" s="36">
         <f>'Data Latih'!I9</f>
         <v>26</v>
       </c>
-      <c r="J9" s="43">
+      <c r="J9" s="36">
         <f>'Data Latih'!J9</f>
         <v>1</v>
       </c>
-      <c r="K9" s="43" t="str">
+      <c r="K9" s="36" t="str">
         <f>'Data Latih'!K9</f>
         <v>Ringan</v>
       </c>
-      <c r="L9" s="45" t="str">
+      <c r="L9" s="38" t="str">
         <f>Distance!$AE$13</f>
         <v>Berat</v>
       </c>
@@ -3439,51 +3441,51 @@
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A10" s="44">
+      <c r="A10" s="37">
         <f>Normalisasi!$A10</f>
         <v>9</v>
       </c>
-      <c r="B10" s="43">
+      <c r="B10" s="36">
         <f>'Data Latih'!B10</f>
         <v>2</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="36">
         <f>'Data Latih'!C10</f>
         <v>2</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="36">
         <f>'Data Latih'!D10</f>
         <v>2</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="36">
         <f>'Data Latih'!E10</f>
         <v>2</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="36">
         <f>'Data Latih'!F10</f>
         <v>1</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="36">
         <f>'Data Latih'!G10</f>
         <v>3</v>
       </c>
-      <c r="H10" s="43">
+      <c r="H10" s="36">
         <f>'Data Latih'!H10</f>
         <v>2</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="36">
         <f>'Data Latih'!I10</f>
         <v>30</v>
       </c>
-      <c r="J10" s="43">
+      <c r="J10" s="36">
         <f>'Data Latih'!J10</f>
         <v>1</v>
       </c>
-      <c r="K10" s="56" t="str">
+      <c r="K10" s="49" t="str">
         <f>'Data Latih'!K10</f>
         <v>Berat</v>
       </c>
-      <c r="L10" s="57" t="str">
+      <c r="L10" s="50" t="str">
         <f>Distance!$AI$13</f>
         <v>Berat</v>
       </c>
@@ -3496,51 +3498,51 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="46">
+      <c r="A11" s="39">
         <f>Normalisasi!$A11</f>
         <v>10</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B11" s="40">
         <f>'Data Latih'!B11</f>
         <v>2</v>
       </c>
-      <c r="C11" s="47">
+      <c r="C11" s="40">
         <f>'Data Latih'!C11</f>
         <v>1</v>
       </c>
-      <c r="D11" s="47">
+      <c r="D11" s="40">
         <f>'Data Latih'!D11</f>
         <v>2</v>
       </c>
-      <c r="E11" s="47">
+      <c r="E11" s="40">
         <f>'Data Latih'!E11</f>
         <v>1</v>
       </c>
-      <c r="F11" s="47">
+      <c r="F11" s="40">
         <f>'Data Latih'!F11</f>
         <v>1</v>
       </c>
-      <c r="G11" s="47">
+      <c r="G11" s="40">
         <f>'Data Latih'!G11</f>
         <v>1</v>
       </c>
-      <c r="H11" s="47">
+      <c r="H11" s="40">
         <f>'Data Latih'!H11</f>
         <v>1</v>
       </c>
-      <c r="I11" s="47">
+      <c r="I11" s="40">
         <f>'Data Latih'!I11</f>
         <v>28</v>
       </c>
-      <c r="J11" s="47">
+      <c r="J11" s="40">
         <f>'Data Latih'!J11</f>
         <v>3</v>
       </c>
-      <c r="K11" s="47" t="str">
+      <c r="K11" s="40" t="str">
         <f>'Data Latih'!K11</f>
         <v>Ringan</v>
       </c>
-      <c r="L11" s="45" t="str">
+      <c r="L11" s="38" t="str">
         <f>Distance!$AM$13</f>
         <v>Berat</v>
       </c>
@@ -3603,14 +3605,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB25C7D-B0BB-4B3F-8B97-9BA2392472ED}">
   <dimension ref="A1:AM15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
     <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.21875" style="6" customWidth="1"/>
     <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
@@ -3639,57 +3641,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="57"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="39"/>
-      <c r="I1" s="37" t="s">
+      <c r="F1" s="56"/>
+      <c r="G1" s="57"/>
+      <c r="I1" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="39"/>
-      <c r="M1" s="37" t="s">
+      <c r="J1" s="56"/>
+      <c r="K1" s="57"/>
+      <c r="M1" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="38"/>
-      <c r="O1" s="39"/>
-      <c r="Q1" s="37" t="s">
+      <c r="N1" s="56"/>
+      <c r="O1" s="57"/>
+      <c r="Q1" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="38"/>
-      <c r="S1" s="39"/>
-      <c r="U1" s="37" t="s">
+      <c r="R1" s="56"/>
+      <c r="S1" s="57"/>
+      <c r="U1" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="V1" s="38"/>
-      <c r="W1" s="39"/>
-      <c r="Y1" s="37" t="s">
+      <c r="V1" s="56"/>
+      <c r="W1" s="57"/>
+      <c r="Y1" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="39"/>
-      <c r="AC1" s="37" t="s">
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="57"/>
+      <c r="AC1" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="AD1" s="38"/>
-      <c r="AE1" s="39"/>
-      <c r="AG1" s="37" t="s">
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="57"/>
+      <c r="AG1" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="AH1" s="38"/>
-      <c r="AI1" s="39"/>
-      <c r="AK1" s="37" t="s">
+      <c r="AH1" s="56"/>
+      <c r="AI1" s="57"/>
+      <c r="AK1" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="AL1" s="38"/>
-      <c r="AM1" s="39"/>
+      <c r="AL1" s="56"/>
+      <c r="AM1" s="57"/>
     </row>
     <row r="2" spans="1:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="str">
@@ -3808,7 +3810,7 @@
         <f>Normalisasi!$A10</f>
         <v>9</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="53">
         <f>SQRT((Normalisasi!$B10-Normalisasi!$B$2)^2+(Normalisasi!$C10-Normalisasi!$C$2)^2+(Normalisasi!$D10-Normalisasi!$D$2)^2+(Normalisasi!$E10-Normalisasi!$E$2)^2+(Normalisasi!$F10-Normalisasi!$F$2)^2+(Normalisasi!$G10-Normalisasi!$G$2)^2+(Normalisasi!$H10-Normalisasi!$H$2)^2+(Normalisasi!$I10-Normalisasi!$I$2)^2+(Normalisasi!$J10-Normalisasi!$J$2)^2)</f>
         <v>1.4164346021784842</v>
       </c>
@@ -4896,7 +4898,7 @@
         <f>Normalisasi!$A6</f>
         <v>5</v>
       </c>
-      <c r="AH11" s="53">
+      <c r="AH11" s="46">
         <f>SQRT((Normalisasi!$B6-Normalisasi!$B$10)^2+(Normalisasi!$C6-Normalisasi!$C$10)^2+(Normalisasi!$D6-Normalisasi!$D$10)^2+(Normalisasi!$E6-Normalisasi!$E$10)^2+(Normalisasi!$F6-Normalisasi!$F$10)^2+(Normalisasi!$G6-Normalisasi!$G$10)^2+(Normalisasi!$H6-Normalisasi!$H$10)^2+(Normalisasi!$I6-Normalisasi!$I$10)^2+(Normalisasi!$J6-Normalisasi!$J$10)^2)</f>
         <v>2.3028795969111848</v>
       </c>
@@ -4974,7 +4976,7 @@
         <v>27</v>
       </c>
       <c r="AE13" t="str">
-        <f t="shared" ref="AE13:AM13" si="0">IF(COUNTIF(AE$3:AE$5,"Berat")&gt;COUNTIF(AE$3:AE$5,"Ringan"),"Berat","Ringan")</f>
+        <f>IF(COUNTIF(AE$3:AE$5,"Berat")&gt;COUNTIF(AE$3:AE$5,"Ringan"),"Berat","Ringan")</f>
         <v>Berat</v>
       </c>
       <c r="AH13" t="s">
@@ -4988,7 +4990,7 @@
         <v>27</v>
       </c>
       <c r="AM13" t="str">
-        <f t="shared" ref="AM13" si="1">IF(COUNTIF(AM$3:AM$5,"Berat")&gt;COUNTIF(AM$3:AM$5,"Ringan"),"Berat","Ringan")</f>
+        <f>IF(COUNTIF(AM$3:AM$5,"Berat")&gt;COUNTIF(AM$3:AM$5,"Ringan"),"Berat","Ringan")</f>
         <v>Berat</v>
       </c>
     </row>
@@ -5027,8 +5029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29237897-EA30-4407-8893-08511BA1AE99}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5078,11 +5080,11 @@
         <f>'Data Latih'!Q3</f>
         <v>1 = Tidak, 2 = Iya</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="41"/>
-      <c r="I3" s="42"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="60"/>
       <c r="L3">
         <v>1</v>
       </c>
@@ -5122,7 +5124,7 @@
       </c>
       <c r="M4" s="28">
         <f t="shared" ref="M4:M12" si="1">SQRT(((B$26-B17)^2)+((C$26-C17)^2)+((D$26-D17)^2)+((E$26-E17)^2)+((F$26-F17)^2)+((G$26-G17)^2)+((H$26-H17)^2)+((I$26-I17)^2)+((J$26-J17)^2))</f>
-        <v>2.0616391533379468</v>
+        <v>2.0634182017430938</v>
       </c>
       <c r="N4" t="str">
         <f t="shared" si="0"/>
@@ -5145,7 +5147,7 @@
       </c>
       <c r="H5" s="31">
         <f>SMALL($M$3:$M$12,G5)</f>
-        <v>1.5042659168964125</v>
+        <v>1.5102247187550639</v>
       </c>
       <c r="I5" s="32" t="str">
         <f>VLOOKUP(H5,$M$3:$N$12,2,FALSE)</f>
@@ -5156,7 +5158,7 @@
       </c>
       <c r="M5" s="28">
         <f t="shared" si="1"/>
-        <v>2.485146332953216</v>
+        <v>2.4861729041740159</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" si="0"/>
@@ -5179,7 +5181,7 @@
       </c>
       <c r="H6" s="31">
         <f t="shared" ref="H6:H14" si="2">SMALL($M$3:$M$12,G6)</f>
-        <v>1.5118200480217774</v>
+        <v>1.5199757413301278</v>
       </c>
       <c r="I6" s="32" t="str">
         <f t="shared" ref="I6:I14" si="3">VLOOKUP(H6,$M$3:$N$12,2,FALSE)</f>
@@ -5190,7 +5192,7 @@
       </c>
       <c r="M6" s="28">
         <f t="shared" si="1"/>
-        <v>1.5042659168964125</v>
+        <v>1.5102247187550639</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="0"/>
@@ -5213,7 +5215,7 @@
       </c>
       <c r="H7" s="31">
         <f t="shared" si="2"/>
-        <v>1.895029191188742</v>
+        <v>1.9034481355044186</v>
       </c>
       <c r="I7" s="32" t="str">
         <f t="shared" si="3"/>
@@ -5224,7 +5226,7 @@
       </c>
       <c r="M7" s="28">
         <f t="shared" si="1"/>
-        <v>2.0014234877246975</v>
+        <v>2.0049185441630391</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="0"/>
@@ -5247,7 +5249,7 @@
       </c>
       <c r="H8" s="31">
         <f t="shared" si="2"/>
-        <v>1.895029191188742</v>
+        <v>1.9034481355044186</v>
       </c>
       <c r="I8" s="32" t="str">
         <f t="shared" si="3"/>
@@ -5258,7 +5260,7 @@
       </c>
       <c r="M8" s="28">
         <f t="shared" si="1"/>
-        <v>1.5118200480217774</v>
+        <v>1.5199757413301278</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
@@ -5281,7 +5283,7 @@
       </c>
       <c r="H9" s="31">
         <f t="shared" si="2"/>
-        <v>2.0014234877246975</v>
+        <v>2.0049185441630391</v>
       </c>
       <c r="I9" s="32" t="str">
         <f t="shared" si="3"/>
@@ -5292,7 +5294,7 @@
       </c>
       <c r="M9" s="28">
         <f t="shared" si="1"/>
-        <v>1.895029191188742</v>
+        <v>1.9034481355044186</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" si="0"/>
@@ -5304,7 +5306,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="20">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" t="str">
         <f>'Data Latih'!Q10</f>
@@ -5315,7 +5317,7 @@
       </c>
       <c r="H10" s="31">
         <f t="shared" si="2"/>
-        <v>2.0127751476369187</v>
+        <v>2.0196023061274611</v>
       </c>
       <c r="I10" s="32" t="str">
         <f t="shared" si="3"/>
@@ -5326,7 +5328,7 @@
       </c>
       <c r="M10" s="28">
         <f t="shared" si="1"/>
-        <v>2.0127751476369187</v>
+        <v>2.0196023061274611</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="0"/>
@@ -5349,7 +5351,7 @@
       </c>
       <c r="H11" s="31">
         <f t="shared" si="2"/>
-        <v>2.0616391533379468</v>
+        <v>2.0634182017430938</v>
       </c>
       <c r="I11" s="32" t="str">
         <f t="shared" si="3"/>
@@ -5360,7 +5362,7 @@
       </c>
       <c r="M11" s="28">
         <f t="shared" si="1"/>
-        <v>1.895029191188742</v>
+        <v>1.9034481355044186</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="0"/>
@@ -5391,7 +5393,7 @@
       </c>
       <c r="M12" s="28">
         <f t="shared" si="1"/>
-        <v>2.4636914824906784</v>
+        <v>2.4697617277158033</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="0"/>
@@ -5404,7 +5406,7 @@
       </c>
       <c r="H13" s="31">
         <f t="shared" si="2"/>
-        <v>2.4636914824906784</v>
+        <v>2.4697617277158033</v>
       </c>
       <c r="I13" s="32" t="str">
         <f t="shared" si="3"/>
@@ -5417,7 +5419,7 @@
       </c>
       <c r="H14" s="31">
         <f t="shared" si="2"/>
-        <v>2.485146332953216</v>
+        <v>2.4861729041740159</v>
       </c>
       <c r="I14" s="32" t="str">
         <f t="shared" si="3"/>
@@ -5549,7 +5551,7 @@
       </c>
       <c r="I17">
         <f>('Data Latih'!I3-MIN!I$5)/(MAX!I$5-MIN!I$5)</f>
-        <v>1.8867924528301886E-2</v>
+        <v>8.771929824561403E-2</v>
       </c>
       <c r="J17">
         <f>('Data Latih'!J3-MIN!J$5)/(MAX!J$5-MIN!J$5)</f>
@@ -5594,7 +5596,7 @@
       </c>
       <c r="I18">
         <f>('Data Latih'!I4-MIN!I$5)/(MAX!I$5-MIN!I$5)</f>
-        <v>0.96226415094339623</v>
+        <v>0.96491228070175439</v>
       </c>
       <c r="J18">
         <f>('Data Latih'!J4-MIN!J$5)/(MAX!J$5-MIN!J$5)</f>
@@ -5639,7 +5641,7 @@
       </c>
       <c r="I19">
         <f>('Data Latih'!I5-MIN!I$5)/(MAX!I$5-MIN!I$5)</f>
-        <v>0.11320754716981132</v>
+        <v>0.17543859649122806</v>
       </c>
       <c r="J19">
         <f>('Data Latih'!J5-MIN!J$5)/(MAX!J$5-MIN!J$5)</f>
@@ -5684,7 +5686,7 @@
       </c>
       <c r="I20">
         <f>('Data Latih'!I6-MIN!I$5)/(MAX!I$5-MIN!I$5)</f>
-        <v>7.5471698113207544E-2</v>
+        <v>0.14035087719298245</v>
       </c>
       <c r="J20">
         <f>('Data Latih'!J6-MIN!J$5)/(MAX!J$5-MIN!J$5)</f>
@@ -5729,7 +5731,7 @@
       </c>
       <c r="I21">
         <f>('Data Latih'!I7-MIN!I$5)/(MAX!I$5-MIN!I$5)</f>
-        <v>0.18867924528301888</v>
+        <v>0.24561403508771928</v>
       </c>
       <c r="J21">
         <f>('Data Latih'!J7-MIN!J$5)/(MAX!J$5-MIN!J$5)</f>
@@ -5774,7 +5776,7 @@
       </c>
       <c r="I22">
         <f>('Data Latih'!I8-MIN!I$5)/(MAX!I$5-MIN!I$5)</f>
-        <v>0.30188679245283018</v>
+        <v>0.35087719298245612</v>
       </c>
       <c r="J22">
         <f>('Data Latih'!J8-MIN!J$5)/(MAX!J$5-MIN!J$5)</f>
@@ -5819,7 +5821,7 @@
       </c>
       <c r="I23">
         <f>('Data Latih'!I9-MIN!I$5)/(MAX!I$5-MIN!I$5)</f>
-        <v>0.22641509433962265</v>
+        <v>0.2807017543859649</v>
       </c>
       <c r="J23">
         <f>('Data Latih'!J9-MIN!J$5)/(MAX!J$5-MIN!J$5)</f>
@@ -5864,7 +5866,7 @@
       </c>
       <c r="I24">
         <f>('Data Latih'!I10-MIN!I$5)/(MAX!I$5-MIN!I$5)</f>
-        <v>0.30188679245283018</v>
+        <v>0.35087719298245612</v>
       </c>
       <c r="J24">
         <f>('Data Latih'!J10-MIN!J$5)/(MAX!J$5-MIN!J$5)</f>
@@ -5909,7 +5911,7 @@
       </c>
       <c r="I25">
         <f>('Data Latih'!I11-MIN!I$5)/(MAX!I$5-MIN!I$5)</f>
-        <v>0.26415094339622641</v>
+        <v>0.31578947368421051</v>
       </c>
       <c r="J25">
         <f>('Data Latih'!J11-MIN!J$5)/(MAX!J$5-MIN!J$5)</f>

</xml_diff>